<commit_message>
can save and load shopping lists
</commit_message>
<xml_diff>
--- a/grocery.xlsx
+++ b/grocery.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Documents/ShoppingHelper/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBCDCB2-4756-DD48-9CC8-2BA565C403B9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="14540" windowWidth="25600" xWindow="0" yWindow="460"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="List2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>Bananas</t>
   </si>
@@ -79,21 +74,22 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
+      <name val="Arial"/>
+      <color rgb="FF000000"/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
     </font>
     <font>
+      <name val="Arial"/>
       <sz val="10"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -109,25 +105,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -427,211 +414,241 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" customHeight="1" defaultColWidth="14.5" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="15.75" r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="1" t="n">
         <v>1.39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="15.75" r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="n">
         <v>6.99</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="15.75" r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="1" t="n">
         <v>6.99</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="15.75" r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="1" t="n">
         <v>6.99</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="15.75" r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="1" t="n">
         <v>4.99</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="15.75" r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1" t="n">
         <v>5.49</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="15.75" r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="1" t="n">
         <v>6.49</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="15.75" r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="1" t="n">
         <v>9.69</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="15.75" r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="1" t="n">
         <v>9.69</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="15.75" r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="1" t="n">
         <v>7.99</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="15.75" r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="1" t="n">
         <v>19.59</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="15.75" r="12" spans="1:2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="n">
         <v>15.79</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="15.75" r="13" spans="1:2">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="1">
-        <v>18.670000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="1" t="n">
+        <v>18.67</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="14" spans="1:2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="1" t="n">
         <v>18.75</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="15.75" r="15" spans="1:2">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="n">
         <v>5.99</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="15.75" r="16" spans="1:2">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="1" t="n">
         <v>6.49</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="15.75" r="17" spans="1:2">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="1" t="n">
         <v>3.66</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="15.75" r="18" spans="1:2">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="1">
-        <v>4.8899999999999997</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="1" t="n">
+        <v>4.89</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="19" spans="1:2">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="n">
         <v>6.29</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="15.75" r="20" spans="1:2">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="1" t="n">
         <v>5.99</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="15.75" r="21" spans="1:2">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="1" t="n">
         <v>4.49</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="15.75" r="22" spans="1:2">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="1">
-        <v>8.7899999999999991</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="1" t="n">
+        <v>8.789999999999999</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="23" spans="1:2">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="1" t="n">
         <v>1.39</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="15.75" r="24" spans="1:2">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="1" t="n">
         <v>6.89</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>